<commit_message>
edit radio button size
</commit_message>
<xml_diff>
--- a/bugs.xlsx
+++ b/bugs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>شماره پورت، اول خالیه</t>
   </si>
@@ -23,9 +23,6 @@
   </si>
   <si>
     <t>سنسور نوری کار نمیکنه</t>
-  </si>
-  <si>
-    <t>رادیو باتن ها خیلی کوچیکن</t>
   </si>
   <si>
     <t>ایرادات کلی</t>
@@ -401,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -415,10 +412,10 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -426,7 +423,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -441,7 +438,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -459,13 +456,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:10" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
     </row>
@@ -475,12 +472,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J13" s="1"/>
+      <c r="J12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>